<commit_message>
excessive reporting for nectar useful graphs of uptake of the ark
git-svn-id: https://ark-informatics.googlecode.com/svn/ARK/trunk@8654 2beaffb7-5388-1629-0768-26d37724f1fc
</commit_message>
<xml_diff>
--- a/usefulTools/Annexure1AgainWithLotsOfGraphsForEachFieldOverTime.xlsx
+++ b/usefulTools/Annexure1AgainWithLotsOfGraphsForEachFieldOverTime.xlsx
@@ -15319,9 +15319,24 @@
   </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:line3DChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -15338,9 +15353,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15428,9 +15440,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15518,9 +15527,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15608,9 +15614,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15698,9 +15701,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15788,9 +15788,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15878,9 +15875,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -15968,9 +15962,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -16058,9 +16049,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$3:$K$3</c:f>
@@ -16142,11 +16130,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="2089512296"/>
         <c:axId val="2083521256"/>
-      </c:lineChart>
+        <c:axId val="2091293912"/>
+      </c:line3DChart>
       <c:catAx>
         <c:axId val="2089512296"/>
         <c:scaling>
@@ -16180,6 +16167,18 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:serAx>
+        <c:axId val="2091293912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2083521256"/>
+      </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -16188,6 +16187,873 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Established Support Tools &amp; Processes (Linked to Funding Milestone 2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integrated existing application with AAF Authentication Services (Linked to Funding Milestone 2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integrated Invoicing &amp; Billing Complete (Linked to Funding Milestone 3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Initial Production Research Cloud Deployed (Linked to Funding Milestone 3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implemented Data Extraction for Analysis Module (Linked to Funding Milestone 4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implemented Pedigree Storage &amp; Visualisation Module (Linked to Funding Milestone 4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enhanced Data Linkage &amp; Reporting Module Complete (Linked to Funding Milestone 5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Implemented Registry Management Module (Linked to Funding Milestone 5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Integrated Genotypic Data Management Capability (Linked to Funding Milestone 5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6/1/12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29-Jun-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27-Jul-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31-Aug-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-Nov-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/31/13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/30/13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9/30/13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/31/13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$12:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2142782536"/>
+        <c:axId val="2142753592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2142782536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142753592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2142753592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142782536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -16225,6 +17091,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -18476,8 +19372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K12" sqref="B3:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added subject and biospec count graphs
git-svn-id: svn://localhost/ARK/trunk@8656 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/Annexure1AgainWithLotsOfGraphsForEachFieldOverTime.xlsx
+++ b/usefulTools/Annexure1AgainWithLotsOfGraphsForEachFieldOverTime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="0" windowWidth="27900" windowHeight="17560" tabRatio="645" activeTab="1"/>
+    <workbookView xWindow="400" yWindow="0" windowWidth="27900" windowHeight="17560" tabRatio="645" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUsers" sheetId="1" r:id="rId1"/>
@@ -17377,6 +17377,27 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Subject (particiants) stored</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -17391,11 +17412,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>subjectCounts!$B$7</c:f>
+              <c:f>subjectCounts!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Initial Production Research Cloud Deployed (Linked to Funding Milestone 3)</c:v>
+                  <c:v>Established Support Tools &amp; Processes (Linked to Funding Milestone 2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17440,7 +17461,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>subjectCounts!$C$7:$K$7</c:f>
+              <c:f>subjectCounts!$C$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17457,19 +17478,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>25000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>32500.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32290.0</c:v>
+                  <c:v>45000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46000.0</c:v>
+                  <c:v>45000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46500.0</c:v>
+                  <c:v>55000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17554,6 +17575,31 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Subject (particiants) stored</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -17618,93 +17664,6 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>61.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Integrated existing application with AAF Authentication Services (Linked to Funding Milestone 2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$5:$K$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -17717,628 +17676,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>25000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>32500.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.0</c:v>
+                  <c:v>45000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.0</c:v>
+                  <c:v>45000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Integrated Invoicing &amp; Billing Complete (Linked to Funding Milestone 3)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$6:$K$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Initial Production Research Cloud Deployed (Linked to Funding Milestone 3)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$7:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32290.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>46500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Implemented Data Extraction for Analysis Module (Linked to Funding Milestone 4)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$8:$K$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>56.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Implemented Pedigree Storage &amp; Visualisation Module (Linked to Funding Milestone 4)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$9:$K$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Enhanced Data Linkage &amp; Reporting Module Complete (Linked to Funding Milestone 5)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$10:$K$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Implemented Registry Management Module (Linked to Funding Milestone 5)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$11:$K$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>61.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>subjectCounts!$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Integrated Genotypic Data Management Capability (Linked to Funding Milestone 5)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>subjectCounts!$C$3:$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>6/1/12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29-Jun-12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27-Jul-12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31-Aug-12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30-Nov-12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/31/13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6/30/13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9/30/13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12/31/13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>subjectCounts!$C$12:$K$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>55000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18353,11 +17703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2139896216"/>
-        <c:axId val="2095699304"/>
+        <c:axId val="-2145432168"/>
+        <c:axId val="2143779032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139896216"/>
+        <c:axId val="-2145432168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18366,7 +17716,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095699304"/>
+        <c:crossAx val="2143779032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18374,7 +17724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095699304"/>
+        <c:axId val="2143779032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18385,7 +17735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139896216"/>
+        <c:crossAx val="-2145432168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18396,7 +17746,7 @@
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -18578,19 +17928,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -21387,7 +20737,7 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="M6" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B12" workbookViewId="0">
       <selection activeCell="R26" sqref="R26:R28"/>
     </sheetView>
   </sheetViews>
@@ -22335,7 +21685,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="L12" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22657,7 +22007,9 @@
       <c r="Q20" s="62">
         <v>45000</v>
       </c>
-      <c r="R20" s="63"/>
+      <c r="R20" s="63">
+        <v>45000</v>
+      </c>
     </row>
     <row r="21" spans="2:18" ht="28" customHeight="1">
       <c r="B21" s="56">
@@ -23291,8 +22643,8 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -23612,7 +22964,9 @@
         <v>29</v>
       </c>
       <c r="Q20" s="62"/>
-      <c r="R20" s="63"/>
+      <c r="R20" s="63">
+        <v>55000</v>
+      </c>
     </row>
     <row r="21" spans="2:18" ht="28" customHeight="1">
       <c r="B21" s="56">
@@ -24247,7 +23601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -24490,8 +23844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24609,40 +23963,40 @@
         <v>Established Support Tools &amp; Processes (Linked to Funding Milestone 2)</v>
       </c>
       <c r="C4">
-        <f>'1'!$H20</f>
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <f>'2'!$H20</f>
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <f>'3'!$H20</f>
-        <v>5</v>
+        <f>'1'!$R$20</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f>'2'!$R$20</f>
+        <v>&gt;1000</v>
+      </c>
+      <c r="E4" t="str">
+        <f>'3'!$R$20</f>
+        <v>&gt;1000</v>
       </c>
       <c r="F4">
-        <f>'4'!$H20</f>
-        <v>5</v>
+        <f>'4'!$R$20</f>
+        <v>0</v>
       </c>
       <c r="G4">
-        <f>'5'!$H20</f>
-        <v>5</v>
+        <f>'5'!$R$20</f>
+        <v>25000</v>
       </c>
       <c r="H4">
-        <f>'6'!$H20</f>
-        <v>15</v>
+        <f>'6'!$R$20</f>
+        <v>32500</v>
       </c>
       <c r="I4">
-        <f>'7'!$H20</f>
-        <v>35</v>
+        <f>'7'!$R$20</f>
+        <v>45000</v>
       </c>
       <c r="J4">
-        <f>'8'!$H20</f>
-        <v>60</v>
+        <f>'8'!$R$20</f>
+        <v>45000</v>
       </c>
       <c r="K4">
-        <f>'9'!$H20</f>
-        <v>61</v>
+        <f>'9'!$R$20</f>
+        <v>55000</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -24653,42 +24007,6 @@
         <f>('1'!C21)</f>
         <v>Integrated existing application with AAF Authentication Services (Linked to Funding Milestone 2)</v>
       </c>
-      <c r="C5">
-        <f>'1'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>'2'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>'3'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f>'4'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f>'5'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>'6'!$H21</f>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>'7'!$H21</f>
-        <v>35</v>
-      </c>
-      <c r="J5">
-        <f>'8'!$H21</f>
-        <v>60</v>
-      </c>
-      <c r="K5">
-        <f>'9'!$H21</f>
-        <v>61</v>
-      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
@@ -24698,42 +24016,6 @@
         <f>('1'!C22)</f>
         <v>Integrated Invoicing &amp; Billing Complete (Linked to Funding Milestone 3)</v>
       </c>
-      <c r="C6">
-        <f>'1'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f>'2'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>'3'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f>'4'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f>'5'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f>'6'!$H22</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f>'7'!$H22</f>
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <f>'8'!$H22</f>
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <f>'9'!$H22</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
@@ -24743,42 +24025,6 @@
         <f>('1'!C23)</f>
         <v>Initial Production Research Cloud Deployed (Linked to Funding Milestone 3)</v>
       </c>
-      <c r="C7">
-        <f>'1'!$N$23</f>
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f>'2'!$N$23</f>
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f>'3'!$N$23</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>'4'!$N$23</f>
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f>'5'!$N$23</f>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>'6'!$N$23</f>
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <f>'7'!$N$23</f>
-        <v>32290</v>
-      </c>
-      <c r="J7">
-        <f>'8'!$N$23</f>
-        <v>46000</v>
-      </c>
-      <c r="K7">
-        <f>'9'!$N$23</f>
-        <v>46500</v>
-      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
@@ -24788,42 +24034,6 @@
         <f>('1'!C24)</f>
         <v>Implemented Data Extraction for Analysis Module (Linked to Funding Milestone 4)</v>
       </c>
-      <c r="C8">
-        <f>'1'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f>'2'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>'3'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f>'4'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>'5'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f>'6'!$H24</f>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>'7'!$H24</f>
-        <v>35</v>
-      </c>
-      <c r="J8">
-        <f>'8'!$H24</f>
-        <v>55</v>
-      </c>
-      <c r="K8">
-        <f>'9'!$H24</f>
-        <v>56</v>
-      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
@@ -24833,42 +24043,6 @@
         <f>('1'!C25)</f>
         <v>Implemented Pedigree Storage &amp; Visualisation Module (Linked to Funding Milestone 4)</v>
       </c>
-      <c r="C9">
-        <f>'1'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f>'2'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>'3'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f>'4'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>'5'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>'6'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f>'7'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f>'8'!$H25</f>
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f>'9'!$H25</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
@@ -24878,42 +24052,6 @@
         <f>('1'!C26)</f>
         <v>Enhanced Data Linkage &amp; Reporting Module Complete (Linked to Funding Milestone 5)</v>
       </c>
-      <c r="C10">
-        <f>'1'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f>'2'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>'3'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f>'4'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>'5'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f>'6'!$H26</f>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f>'7'!$H26</f>
-        <v>35</v>
-      </c>
-      <c r="J10">
-        <f>'8'!$H26</f>
-        <v>60</v>
-      </c>
-      <c r="K10">
-        <f>'9'!$H26</f>
-        <v>6</v>
-      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
@@ -24923,42 +24061,6 @@
         <f>('1'!C27)</f>
         <v>Implemented Registry Management Module (Linked to Funding Milestone 5)</v>
       </c>
-      <c r="C11">
-        <f>'1'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>'2'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>'3'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>'4'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>'5'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>'6'!$H27</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>'7'!$H27</f>
-        <v>35</v>
-      </c>
-      <c r="J11">
-        <f>'8'!$H27</f>
-        <v>60</v>
-      </c>
-      <c r="K11">
-        <f>'9'!$H27</f>
-        <v>61</v>
-      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
@@ -24967,42 +24069,6 @@
       <c r="B12" t="str">
         <f>('1'!C28)</f>
         <v>Integrated Genotypic Data Management Capability (Linked to Funding Milestone 5)</v>
-      </c>
-      <c r="C12">
-        <f>'1'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f>'2'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>'3'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f>'4'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>'5'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f>'6'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f>'7'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f>'8'!$H28</f>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f>'9'!$H28</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -25791,7 +24857,7 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
@@ -27316,7 +26382,7 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C10" workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
@@ -30368,7 +29434,7 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D26" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>